<commit_message>
fix bugs associated with losses calculation
</commit_message>
<xml_diff>
--- a/Input/Training/TIMESERIES/DA_RESERVES.xlsx
+++ b/Input/Training/TIMESERIES/DA_RESERVES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\pikr001\fresh\FESTIV_MODEL\Input\Training\TIMESERIES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD944B5-B0CC-4470-B03F-C9BAF4F5C1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A87CDF3-1B77-4B16-B650-C9142553DC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10215" yWindow="1980" windowWidth="27225" windowHeight="13065" xr2:uid="{3D06E83E-A3EE-4B22-AC2F-DD2AA57403AF}"/>
+    <workbookView xWindow="9480" yWindow="1545" windowWidth="27225" windowHeight="13065" xr2:uid="{3D06E83E-A3EE-4B22-AC2F-DD2AA57403AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,7 +411,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9440C79A-9A8A-4B84-A956-A9C170D4DECC}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -834,10 +836,10 @@
         <v>149.65379999999999</v>
       </c>
       <c r="E21">
-        <v>99.769199999999998</v>
+        <v>96.769199999999998</v>
       </c>
       <c r="F21">
-        <v>99.769199999999998</v>
+        <v>96.769199999999998</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>